<commit_message>
Complete CrossValid & Proportion
</commit_message>
<xml_diff>
--- a/output/comment_robust_jaccard.xlsx
+++ b/output/comment_robust_jaccard.xlsx
@@ -19,22 +19,22 @@
     <t>เมจิ</t>
   </si>
   <si>
-    <t>ไทยเดนมาร์ค</t>
+    <t>ดัชมิลล์</t>
+  </si>
+  <si>
+    <t>โฟร์โมสต์</t>
   </si>
   <si>
     <t>แดรี่โฮม</t>
   </si>
   <si>
-    <t>โฟร์โมสต์</t>
-  </si>
-  <si>
     <t>โชคชัย</t>
   </si>
   <si>
-    <t>หนองโพ</t>
+    <t>เอ็มมิลค์</t>
   </si>
   <si>
-    <t>เอ็มมิลค์</t>
+    <t>ไทยเดนมาร์ค</t>
   </si>
 </sst>
 </file>
@@ -426,25 +426,25 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.6818181818181818</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0.03856470855331604</v>
+        <v>0.1108032196764444</v>
       </c>
       <c r="D2">
-        <v>0.01354644855317492</v>
+        <v>0.09446707970288731</v>
       </c>
       <c r="E2">
-        <v>0.07131459894116972</v>
+        <v>0.01956254241693767</v>
       </c>
       <c r="F2">
-        <v>0.02026939848259975</v>
+        <v>0.02964585807536208</v>
       </c>
       <c r="G2">
-        <v>0.02490677666299386</v>
+        <v>0.04017087007589609</v>
       </c>
       <c r="H2">
-        <v>0.02751095950652278</v>
+        <v>0.05003973575996431</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -452,25 +452,25 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.03856470855331604</v>
+        <v>0.1108032196764444</v>
       </c>
       <c r="C3">
-        <v>0.593939393939394</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0.02584364978545007</v>
+        <v>0.124671961322111</v>
       </c>
       <c r="E3">
-        <v>0.08201110659943436</v>
+        <v>0.02189330424219897</v>
       </c>
       <c r="F3">
-        <v>0.01558692662476912</v>
+        <v>0.04173466467630537</v>
       </c>
       <c r="G3">
-        <v>0.1127041663607508</v>
+        <v>0.0004553734061930783</v>
       </c>
       <c r="H3">
-        <v>2.942041776993233e-05</v>
+        <v>0.1114107448998216</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -478,25 +478,25 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.01354644855317492</v>
+        <v>0.09446707970288731</v>
       </c>
       <c r="C4">
-        <v>0.02584364978545007</v>
+        <v>0.124671961322111</v>
       </c>
       <c r="D4">
-        <v>0.3151515151515151</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.005926161000787866</v>
+        <v>0.03547041304011841</v>
       </c>
       <c r="G4">
-        <v>0.01611960974762261</v>
+        <v>0.0002579979360165118</v>
       </c>
       <c r="H4">
-        <v>0.001388888888888889</v>
+        <v>0.117420824480639</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -504,25 +504,25 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.07131459894116972</v>
+        <v>0.01956254241693767</v>
       </c>
       <c r="C5">
-        <v>0.08201110659943436</v>
+        <v>0.02189330424219897</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.5848484848484848</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>0.02192716442480047</v>
+        <v>0.01346409356032294</v>
       </c>
       <c r="G5">
-        <v>0.09304998685617365</v>
+        <v>0.003787878787878788</v>
       </c>
       <c r="H5">
-        <v>0.0001594896331738437</v>
+        <v>0.0426602026144021</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -530,25 +530,25 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.02026939848259975</v>
+        <v>0.02964585807536208</v>
       </c>
       <c r="C6">
-        <v>0.01558692662476912</v>
+        <v>0.04173466467630537</v>
       </c>
       <c r="D6">
-        <v>0.005926161000787866</v>
+        <v>0.03547041304011841</v>
       </c>
       <c r="E6">
-        <v>0.02192716442480047</v>
+        <v>0.01346409356032294</v>
       </c>
       <c r="F6">
-        <v>0.3393939393939394</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>0.009850784318738965</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>0.02487639490014739</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -556,25 +556,25 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.02490677666299386</v>
+        <v>0.04017087007589609</v>
       </c>
       <c r="C7">
-        <v>0.1127041663607508</v>
+        <v>0.0004553734061930783</v>
       </c>
       <c r="D7">
-        <v>0.01611960974762261</v>
+        <v>0.0002579979360165118</v>
       </c>
       <c r="E7">
-        <v>0.09304998685617365</v>
+        <v>0.003787878787878788</v>
       </c>
       <c r="F7">
-        <v>0.009850784318738965</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0.4303030303030303</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>4.782629489693433e-05</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -582,25 +582,25 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.02751095950652278</v>
+        <v>0.05003973575996431</v>
       </c>
       <c r="C8">
-        <v>2.942041776993233e-05</v>
+        <v>0.1114107448998216</v>
       </c>
       <c r="D8">
-        <v>0.001388888888888889</v>
+        <v>0.117420824480639</v>
       </c>
       <c r="E8">
-        <v>0.0001594896331738437</v>
+        <v>0.0426602026144021</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.02487639490014739</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>4.782629489693433e-05</v>
       </c>
       <c r="H8">
-        <v>0.1636363636363636</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>